<commit_message>
Deploying to gh-pages from  @ 42bd8da80e6e68c47101f55a924ece5bac27bfc4 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/2.1.2.xlsx
+++ b/en/downloads/data-excel/2.1.2.xlsx
@@ -191,7 +191,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="###0.0"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +300,37 @@
       <i/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman Cyr"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman Cyr"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -351,7 +386,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -359,8 +394,9 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -469,13 +505,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1"/>
     <cellStyle name="Обычный 2 2" xfId="2"/>
     <cellStyle name="Обычный 3" xfId="3"/>
     <cellStyle name="Обычный 4" xfId="6"/>
+    <cellStyle name="Обычный_Лист2" xfId="7"/>
     <cellStyle name="Процентный 2" xfId="5"/>
     <cellStyle name="Процентный 3" xfId="4"/>
   </cellStyles>
@@ -779,11 +822,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +836,7 @@
     <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="8" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>56</v>
       </c>
@@ -804,7 +847,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -815,8 +858,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -832,8 +875,11 @@
       <c r="E4" s="13">
         <v>2020</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="13">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>54</v>
       </c>
@@ -846,7 +892,7 @@
       <c r="D5" s="32"/>
       <c r="E5" s="32"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
@@ -862,8 +908,11 @@
       <c r="E6" s="33">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="40">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>36</v>
       </c>
@@ -875,8 +924,9 @@
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="40"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>42</v>
       </c>
@@ -892,8 +942,11 @@
       <c r="E8" s="34">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="41">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>45</v>
       </c>
@@ -909,8 +962,11 @@
       <c r="E9" s="34">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="41">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>39</v>
       </c>
@@ -922,8 +978,9 @@
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
-    </row>
-    <row r="11" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="42"/>
+    </row>
+    <row r="11" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -939,8 +996,11 @@
       <c r="E11" s="34">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="43">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -956,8 +1016,11 @@
       <c r="E12" s="34">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="41">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -973,8 +1036,11 @@
       <c r="E13" s="34">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="41">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -990,8 +1056,11 @@
       <c r="E14" s="34">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="41">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1007,8 +1076,11 @@
       <c r="E15" s="34">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="41">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1024,8 +1096,11 @@
       <c r="E16" s="34">
         <v>7.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="41">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1041,8 +1116,11 @@
       <c r="E17" s="34">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="41">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -1058,8 +1136,11 @@
       <c r="E18" s="34">
         <v>10.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="41">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>27</v>
       </c>
@@ -1075,8 +1156,11 @@
       <c r="E19" s="34">
         <v>12.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="41">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>55</v>
       </c>
@@ -1089,7 +1173,7 @@
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>2</v>
       </c>
@@ -1105,8 +1189,11 @@
       <c r="E21" s="36">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="40">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>36</v>
       </c>
@@ -1118,8 +1205,9 @@
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="40"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
@@ -1135,8 +1223,11 @@
       <c r="E23" s="34">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="41">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>45</v>
       </c>
@@ -1152,8 +1243,11 @@
       <c r="E24" s="34">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="41">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>39</v>
       </c>
@@ -1165,8 +1259,9 @@
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="42"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
@@ -1182,8 +1277,11 @@
       <c r="E26" s="34">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="43">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1199,8 +1297,11 @@
       <c r="E27" s="34">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="41">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -1216,8 +1317,11 @@
       <c r="E28" s="34">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="41">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -1233,8 +1337,11 @@
       <c r="E29" s="34">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="41">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -1250,8 +1357,11 @@
       <c r="E30" s="34">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="41">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>18</v>
       </c>
@@ -1267,8 +1377,11 @@
       <c r="E31" s="34">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -1284,8 +1397,11 @@
       <c r="E32" s="34">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>24</v>
       </c>
@@ -1301,8 +1417,11 @@
       <c r="E33" s="34">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="41">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>27</v>
       </c>
@@ -1317,6 +1436,9 @@
       </c>
       <c r="E34" s="37">
         <v>3.7</v>
+      </c>
+      <c r="F34" s="37">
+        <v>11.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>